<commit_message>
fix import muc chi vs chung tu
</commit_message>
<xml_diff>
--- a/WebApp/wwwroot/template/TemplateImportActiveGroup.xlsx
+++ b/WebApp/wwwroot/template/TemplateImportActiveGroup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HOME\CreditRequestSystem\WebApp\wwwroot\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\OnGIT\CreditRequestSystem\WebApp\wwwroot\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -64,7 +64,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -388,15 +388,15 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="64" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
add code import for nguon thu vs nhom hoat dong
</commit_message>
<xml_diff>
--- a/WebApp/wwwroot/template/TemplateImportActiveGroup.xlsx
+++ b/WebApp/wwwroot/template/TemplateImportActiveGroup.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\OnGIT\CreditRequestSystem\WebApp\wwwroot\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nghia\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA07D7BA-8F65-40DC-9F22-6A36A942D14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,16 +25,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Tên nhóm hoạt động</t>
+  </si>
+  <si>
+    <t>Mã nhóm hoạt động</t>
+  </si>
+  <si>
+    <t>Nhom001</t>
+  </si>
+  <si>
+    <t>Thể dục thể thao</t>
+  </si>
+  <si>
+    <t>Nhom002</t>
+  </si>
+  <si>
+    <t>Đường lối định hướng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +69,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -96,13 +120,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -384,25 +411,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="64" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="64" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>